<commit_message>
Se cargan los archivos del 3 trimestre y se ordenan los entregables
</commit_message>
<xml_diff>
--- a/proy_formativo/documentacion/2do_Trim/Diccionario de Datos/8 - Plantilla Diccionario de Datos.xlsx
+++ b/proy_formativo/documentacion/2do_Trim/Diccionario de Datos/8 - Plantilla Diccionario de Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\SENA\Proyecto Sena\MER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\SENA\Proyecto Sena\Sistema de Información Gestor-E\proy_formativo\documentacion\2do_Trim\Diccionario de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE709C15-8457-43F8-AF71-C337B65EEA7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77F3932-2539-46AE-932C-F3F3C1CA0051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="0" windowWidth="21600" windowHeight="11385" tabRatio="719" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="315" windowWidth="21600" windowHeight="11355" tabRatio="719" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTRODUCCIÓN" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Campos!$B$2:$L$2</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Bases de Datos'!$A$1:$G$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Campos!$A$1:$Q$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">Campos!$A$1:$Q$52</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Constraints!$A$1:$E$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">INTRODUCCIÓN!$A$1:$J$48</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Objetos!$A$1:$E$17</definedName>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="177">
   <si>
     <t>PROYECTO</t>
   </si>
@@ -771,9 +771,6 @@
     <t>Código GTI-F-010</t>
   </si>
   <si>
-    <t xml:space="preserve">USUARIOS </t>
-  </si>
-  <si>
     <t>(NUMERO)</t>
   </si>
   <si>
@@ -878,9 +875,6 @@
     <t xml:space="preserve">Mysql Workbench </t>
   </si>
   <si>
-    <t xml:space="preserve">Usuarios, Proveedores, Categorias, Productos   </t>
-  </si>
-  <si>
     <t>Desarrollar un sistema de Información que sirva como apoyo al proceso de la gestión de inventarios en la empresa Vitugoz.</t>
   </si>
   <si>
@@ -902,22 +896,10 @@
     <t>Reatiga Otalora</t>
   </si>
   <si>
-    <t>JNC</t>
-  </si>
-  <si>
     <t>En esta tabla se van a consignar los datos de todos los usuarios que van a interactuar con el sistema</t>
   </si>
   <si>
-    <t>PROVEEDORES</t>
-  </si>
-  <si>
     <t xml:space="preserve">En esta tabla se van a consignar los datos de todos los proveedores con los que se tiene alguna relación comercial </t>
-  </si>
-  <si>
-    <t>PRODUCTOS</t>
-  </si>
-  <si>
-    <t>CATEGORIAS</t>
   </si>
   <si>
     <t>En esta tabla se van a consignar los datos de todos los productos que ingresan y/o salen de la compañía</t>
@@ -1070,9 +1052,6 @@
     <t>Atributo para almacenar y verificar el usuario que hizo la creación del producto</t>
   </si>
   <si>
-    <t>CATEGORIA</t>
-  </si>
-  <si>
     <t>CATEGORYID</t>
   </si>
   <si>
@@ -1107,6 +1086,123 @@
   </si>
   <si>
     <t>(VARCHAR80)</t>
+  </si>
+  <si>
+    <t>En esta tabla se almacenarán los roles que se le asignarán a cada usuario del sistema</t>
+  </si>
+  <si>
+    <t>RolID</t>
+  </si>
+  <si>
+    <t>RolName</t>
+  </si>
+  <si>
+    <t>Atributo identificador único de cada Rol</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar nombre del Rol</t>
+  </si>
+  <si>
+    <t>Gestor-E</t>
+  </si>
+  <si>
+    <t>Roles, users, categories, requests, suppliers, products, categories, bills</t>
+  </si>
+  <si>
+    <t>ROLES</t>
+  </si>
+  <si>
+    <t>USERS</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>SUPPLIERS</t>
+  </si>
+  <si>
+    <t>REQUESTS</t>
+  </si>
+  <si>
+    <t>BILLS</t>
+  </si>
+  <si>
+    <t>En esta tabla se almacenarán las solicitudes creadas por cada usuario dentro del sistema</t>
+  </si>
+  <si>
+    <t>En esta tabla quedará almacenada la información básica de cada factura generada por los proveedores</t>
+  </si>
+  <si>
+    <t>RolDescription</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la descripción del Rol</t>
+  </si>
+  <si>
+    <t>RequestId</t>
+  </si>
+  <si>
+    <t>RequestDescription</t>
+  </si>
+  <si>
+    <t>RequestDateStart</t>
+  </si>
+  <si>
+    <t>RequestStatus</t>
+  </si>
+  <si>
+    <t>RequestsAmount</t>
+  </si>
+  <si>
+    <t>RequestDateEnd</t>
+  </si>
+  <si>
+    <t>(VARCHAR90)</t>
+  </si>
+  <si>
+    <t>Atributo identificador único de cada Solicitud</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la descripción de la Solicitud</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la fecha inicial de solicitud</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la fecha final de solicitud</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la el estatus de la solicitud</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la cantidad de la solicitud</t>
+  </si>
+  <si>
+    <t>Billid</t>
+  </si>
+  <si>
+    <t>BillName</t>
+  </si>
+  <si>
+    <t>BillDescription</t>
+  </si>
+  <si>
+    <t>BillDate</t>
+  </si>
+  <si>
+    <t>Atributo identificador único de cada Factura</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar nombre de la Factura</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la descripción de la Factura</t>
+  </si>
+  <si>
+    <t>Atributo para almacenar la fecha de la factura</t>
   </si>
 </sst>
 </file>
@@ -1802,7 +1898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1947,6 +2043,15 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1954,6 +2059,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1964,75 +2078,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2133,6 +2178,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2150,6 +2246,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2562,7 +2664,7 @@
   <dimension ref="B1:I48"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:I44"/>
+      <selection activeCell="C46" sqref="C46:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,402 +2684,402 @@
   <sheetData>
     <row r="1" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="83"/>
-      <c r="C2" s="86" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="79" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="80"/>
+      <c r="I2" s="63"/>
     </row>
     <row r="3" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="84"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="82"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="2:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="85"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="101" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="102"/>
+      <c r="I4" s="85"/>
     </row>
     <row r="5" spans="2:9" s="13" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
     </row>
     <row r="6" spans="2:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="106"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="89"/>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="109"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="111"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="94"/>
     </row>
     <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="95" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="97"/>
+      <c r="C8" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="80"/>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="98" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="100"/>
+      <c r="C9" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="83"/>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="98" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="100"/>
+      <c r="C10" s="81" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="83"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="107"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="108"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="91"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="78"/>
+      <c r="C12" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
     </row>
     <row r="13" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="C13" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="59"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="72"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="59"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="72"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="59"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="72"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="59"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="72"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="59"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="72"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="59"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="55"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="61"/>
     </row>
     <row r="20" spans="2:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="72"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
       <c r="F20" s="14"/>
     </row>
     <row r="21" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="61"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="72"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="61"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="72"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="58"/>
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="61"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="72"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="61"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="72"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="14"/>
     </row>
     <row r="25" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="61"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="72"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="14"/>
     </row>
     <row r="26" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="61"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="72"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="14"/>
     </row>
     <row r="27" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="61"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="72"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="14"/>
     </row>
     <row r="28" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="61"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="72"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="14"/>
     </row>
     <row r="29" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="61"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="72"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="58"/>
       <c r="F29" s="14"/>
     </row>
     <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="61"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="72"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="58"/>
       <c r="F30" s="14"/>
     </row>
     <row r="31" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="61"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="72"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="58"/>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="61"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="72"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="58"/>
       <c r="F32" s="14"/>
     </row>
     <row r="33" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="61"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="72"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="61"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="72"/>
+      <c r="B34" s="100"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="58"/>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="61"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="72"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="58"/>
       <c r="F35" s="14"/>
     </row>
     <row r="36" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="63"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="75"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="110"/>
+      <c r="E36" s="111"/>
       <c r="F36" s="14"/>
     </row>
     <row r="37" spans="2:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="66"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="104"/>
+      <c r="E37" s="105"/>
       <c r="F37" s="14"/>
     </row>
     <row r="38" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="61"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="69"/>
+      <c r="B38" s="100"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="107"/>
+      <c r="E38" s="108"/>
       <c r="F38" s="14"/>
     </row>
     <row r="39" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="61"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="69"/>
+      <c r="B39" s="100"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="108"/>
       <c r="F39" s="14"/>
     </row>
     <row r="40" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="61"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="69"/>
+      <c r="B40" s="100"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="108"/>
       <c r="F40" s="14"/>
     </row>
     <row r="41" spans="2:9" ht="108" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="63"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="69"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="108"/>
       <c r="F41" s="14"/>
     </row>
     <row r="42" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="52"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="55"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="61"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="71"/>
-      <c r="I43" s="72"/>
+      <c r="B43" s="100"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="58"/>
     </row>
     <row r="44" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="62"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="55"/>
+      <c r="B44" s="101"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="61"/>
     </row>
     <row r="45" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="6"/>
@@ -2990,30 +3092,38 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="50"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="52"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54"/>
+      <c r="I46" s="55"/>
     </row>
     <row r="47" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="57"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="55"/>
+      <c r="B47" s="96"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="61"/>
     </row>
     <row r="48" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C46:I47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="C37:E41"/>
+    <mergeCell ref="B20:B36"/>
+    <mergeCell ref="C20:E36"/>
     <mergeCell ref="C12:I12"/>
     <mergeCell ref="C13:I19"/>
     <mergeCell ref="C42:I44"/>
@@ -3028,14 +3138,6 @@
     <mergeCell ref="B6:I6"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B7:I7"/>
-    <mergeCell ref="C46:I47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="C37:E41"/>
-    <mergeCell ref="B20:B36"/>
-    <mergeCell ref="C20:E36"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3050,7 +3152,7 @@
   <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3077,13 +3179,13 @@
     </row>
     <row r="3" spans="2:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3100,8 +3202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:F6"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="D1" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3137,46 +3239,46 @@
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
       <c r="C4" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3193,8 +3295,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B1:F4"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="190" zoomScaleNormal="100" zoomScaleSheetLayoutView="190" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="C1" zoomScale="190" zoomScaleNormal="100" zoomScaleSheetLayoutView="190" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3229,12 +3331,12 @@
     </row>
     <row r="3" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="C3" s="37"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F3" s="17"/>
     </row>
@@ -3255,7 +3357,7 @@
   <dimension ref="B1:D166"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3282,62 +3384,80 @@
     </row>
     <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
-        <v>78</v>
+        <v>149</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="17"/>
+      <c r="B8" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="20"/>
@@ -3393,8 +3513,8 @@
   </sheetPr>
   <dimension ref="B1:Q2368"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A19" zoomScale="80" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="D13" zoomScale="80" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,37 +3542,37 @@
     <row r="1" spans="2:17" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="42" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="42" t="s">
-        <v>59</v>
       </c>
       <c r="J2" s="34" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="34" t="s">
         <v>60</v>
-      </c>
-      <c r="L2" s="34" t="s">
-        <v>61</v>
       </c>
       <c r="M2" s="34" t="s">
         <v>12</v>
@@ -3464,24 +3584,24 @@
         <v>14</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="112" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>34</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>35</v>
       </c>
       <c r="G3" s="45">
         <v>8</v>
@@ -3490,16 +3610,16 @@
         <v>8</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="44">
         <v>0</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
@@ -3509,12 +3629,12 @@
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="113"/>
       <c r="C4" s="44" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
       <c r="F4" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G4" s="44">
         <v>25</v>
@@ -3523,16 +3643,16 @@
         <v>25</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K4" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
@@ -3542,12 +3662,12 @@
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="113"/>
       <c r="C5" s="44" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D5" s="44"/>
       <c r="E5" s="44"/>
       <c r="F5" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G5" s="44">
         <v>25</v>
@@ -3556,16 +3676,16 @@
         <v>25</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J5" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L5" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
@@ -3575,12 +3695,12 @@
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="113"/>
       <c r="C6" s="44" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44"/>
       <c r="F6" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G6" s="44">
         <v>25</v>
@@ -3589,16 +3709,16 @@
         <v>25</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J6" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K6" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L6" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
@@ -3608,12 +3728,12 @@
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="113"/>
       <c r="C7" s="44" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
       <c r="F7" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="44">
         <v>25</v>
@@ -3622,16 +3742,16 @@
         <v>25</v>
       </c>
       <c r="I7" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K7" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L7" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
@@ -3641,12 +3761,12 @@
     <row r="8" spans="2:17" s="28" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="113"/>
       <c r="C8" s="44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="44"/>
       <c r="F8" s="44" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G8" s="44">
         <v>15</v>
@@ -3655,16 +3775,16 @@
         <v>10</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J8" s="43" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="K8" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L8" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
@@ -3674,12 +3794,12 @@
     <row r="9" spans="2:17" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="113"/>
       <c r="C9" s="44" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="44"/>
       <c r="F9" s="44" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G9" s="44">
         <v>20</v>
@@ -3688,16 +3808,16 @@
         <v>20</v>
       </c>
       <c r="I9" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" s="43" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="K9" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
@@ -3707,12 +3827,12 @@
     <row r="10" spans="2:17" s="28" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="113"/>
       <c r="C10" s="44" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="44"/>
       <c r="F10" s="44" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G10" s="44">
         <v>20</v>
@@ -3721,16 +3841,16 @@
         <v>20</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J10" s="43" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="K10" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L10" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
@@ -3740,12 +3860,12 @@
     <row r="11" spans="2:17" s="28" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="113"/>
       <c r="C11" s="44" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="44" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G11" s="44">
         <v>20</v>
@@ -3754,16 +3874,16 @@
         <v>20</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J11" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L11" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
@@ -3773,12 +3893,12 @@
     <row r="12" spans="2:17" s="28" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B12" s="113"/>
       <c r="C12" s="44" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D12" s="44"/>
       <c r="E12" s="44"/>
       <c r="F12" s="44" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G12" s="44">
         <v>20</v>
@@ -3787,16 +3907,16 @@
         <v>20</v>
       </c>
       <c r="I12" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J12" s="43" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="K12" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L12" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
@@ -3806,12 +3926,12 @@
     <row r="13" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="113"/>
       <c r="C13" s="49" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D13" s="44"/>
       <c r="E13" s="44"/>
       <c r="F13" s="44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G13" s="44">
         <v>35</v>
@@ -3820,16 +3940,16 @@
         <v>35</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J13" s="43" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="K13" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
@@ -3839,17 +3959,19 @@
     </row>
     <row r="14" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="112" t="s">
-        <v>78</v>
+        <v>149</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="44"/>
+        <v>39</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" s="44">
         <v>8</v>
@@ -3858,16 +3980,16 @@
         <v>8</v>
       </c>
       <c r="I14" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J14" s="43" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K14" s="44">
         <v>0</v>
       </c>
       <c r="L14" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
@@ -3878,12 +4000,12 @@
     <row r="15" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="113"/>
       <c r="C15" s="44" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D15" s="44"/>
       <c r="E15" s="44"/>
       <c r="F15" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G15" s="44">
         <v>25</v>
@@ -3892,16 +4014,16 @@
         <v>25</v>
       </c>
       <c r="I15" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J15" s="43" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K15" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L15" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
@@ -3912,12 +4034,12 @@
     <row r="16" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="113"/>
       <c r="C16" s="44" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
       <c r="F16" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G16" s="44">
         <v>25</v>
@@ -3926,16 +4048,16 @@
         <v>25</v>
       </c>
       <c r="I16" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J16" s="43" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K16" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L16" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
@@ -3946,12 +4068,12 @@
     <row r="17" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="113"/>
       <c r="C17" s="44" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D17" s="44"/>
       <c r="E17" s="44"/>
       <c r="F17" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="44">
         <v>13</v>
@@ -3960,16 +4082,16 @@
         <v>7</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" s="43" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K17" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L17" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
@@ -3980,12 +4102,12 @@
     <row r="18" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="113"/>
       <c r="C18" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D18" s="44"/>
       <c r="E18" s="44"/>
       <c r="F18" s="44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G18" s="44">
         <v>35</v>
@@ -3994,16 +4116,16 @@
         <v>35</v>
       </c>
       <c r="I18" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J18" s="43" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="K18" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L18" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
@@ -4013,12 +4135,12 @@
     <row r="19" spans="2:17" s="28" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B19" s="113"/>
       <c r="C19" s="44" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D19" s="44"/>
       <c r="E19" s="44"/>
       <c r="F19" s="44" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G19" s="44">
         <v>80</v>
@@ -4027,16 +4149,16 @@
         <v>80</v>
       </c>
       <c r="I19" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J19" s="43" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K19" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
@@ -4046,12 +4168,12 @@
     <row r="20" spans="2:17" s="28" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B20" s="113"/>
       <c r="C20" s="44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D20" s="44"/>
       <c r="E20" s="44"/>
       <c r="F20" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G20" s="44">
         <v>25</v>
@@ -4060,16 +4182,16 @@
         <v>25</v>
       </c>
       <c r="I20" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K20" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L20" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
@@ -4079,12 +4201,12 @@
     <row r="21" spans="2:17" s="28" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="113"/>
       <c r="C21" s="44" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D21" s="44"/>
       <c r="E21" s="44"/>
       <c r="F21" s="44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G21" s="44">
         <v>35</v>
@@ -4093,16 +4215,16 @@
         <v>35</v>
       </c>
       <c r="I21" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J21" s="43" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="K21" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L21" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
@@ -4112,12 +4234,12 @@
     <row r="22" spans="2:17" s="28" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B22" s="113"/>
       <c r="C22" s="44" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D22" s="44"/>
       <c r="E22" s="44"/>
       <c r="F22" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G22" s="44">
         <v>25</v>
@@ -4126,16 +4248,16 @@
         <v>25</v>
       </c>
       <c r="I22" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J22" s="43" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="K22" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L22" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
@@ -4145,26 +4267,26 @@
     <row r="23" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="113"/>
       <c r="C23" s="44" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
       <c r="F23" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
       <c r="I23" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J23" s="43" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K23" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L23" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
@@ -4173,17 +4295,19 @@
     </row>
     <row r="24" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="114" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="44"/>
+        <v>39</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>38</v>
+      </c>
       <c r="F24" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24" s="44">
         <v>8</v>
@@ -4192,16 +4316,16 @@
         <v>8</v>
       </c>
       <c r="I24" s="44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J24" s="43" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="K24" s="44">
         <v>0</v>
       </c>
       <c r="L24" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
@@ -4211,12 +4335,12 @@
     <row r="25" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="114"/>
       <c r="C25" s="44" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D25" s="44"/>
       <c r="E25" s="44"/>
       <c r="F25" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G25" s="44">
         <v>25</v>
@@ -4225,16 +4349,16 @@
         <v>25</v>
       </c>
       <c r="I25" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J25" s="43" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="K25" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L25" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
@@ -4244,12 +4368,12 @@
     <row r="26" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="114"/>
       <c r="C26" s="44" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D26" s="44"/>
       <c r="E26" s="44"/>
       <c r="F26" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G26" s="44">
         <v>12</v>
@@ -4258,16 +4382,16 @@
         <v>12</v>
       </c>
       <c r="I26" s="44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J26" s="43" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K26" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L26" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
@@ -4277,12 +4401,12 @@
     <row r="27" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="114"/>
       <c r="C27" s="44" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D27" s="44"/>
       <c r="E27" s="44"/>
       <c r="F27" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="44">
         <v>5</v>
@@ -4291,16 +4415,16 @@
         <v>5</v>
       </c>
       <c r="I27" s="44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J27" s="43" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L27" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M27" s="22"/>
       <c r="N27" s="22"/>
@@ -4310,12 +4434,12 @@
     <row r="28" spans="2:17" s="28" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B28" s="114"/>
       <c r="C28" s="44" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D28" s="44"/>
       <c r="E28" s="44"/>
       <c r="F28" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G28" s="44">
         <v>25</v>
@@ -4324,16 +4448,16 @@
         <v>25</v>
       </c>
       <c r="I28" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J28" s="43" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K28" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L28" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
@@ -4343,26 +4467,26 @@
     <row r="29" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="114"/>
       <c r="C29" s="44" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
       <c r="F29" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G29" s="46"/>
       <c r="H29" s="46"/>
       <c r="I29" s="44" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J29" s="43" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K29" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L29" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M29" s="30"/>
       <c r="N29" s="22"/>
@@ -4371,17 +4495,19 @@
     </row>
     <row r="30" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="114" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="44"/>
+        <v>39</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>38</v>
+      </c>
       <c r="F30" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G30" s="44">
         <v>8</v>
@@ -4390,16 +4516,16 @@
         <v>8</v>
       </c>
       <c r="I30" s="44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J30" s="43" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="K30" s="44">
         <v>0</v>
       </c>
       <c r="L30" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M30" s="22"/>
       <c r="N30" s="22"/>
@@ -4409,12 +4535,12 @@
     <row r="31" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="114"/>
       <c r="C31" s="44" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D31" s="44"/>
       <c r="E31" s="44"/>
       <c r="F31" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G31" s="44">
         <v>25</v>
@@ -4423,16 +4549,16 @@
         <v>25</v>
       </c>
       <c r="I31" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J31" s="43" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="K31" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L31" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M31" s="30"/>
       <c r="N31" s="22"/>
@@ -4442,12 +4568,12 @@
     <row r="32" spans="2:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="114"/>
       <c r="C32" s="44" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
       <c r="F32" s="44" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G32" s="44">
         <v>80</v>
@@ -4456,16 +4582,16 @@
         <v>80</v>
       </c>
       <c r="I32" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J32" s="43" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="K32" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L32" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M32" s="30"/>
       <c r="N32" s="22"/>
@@ -4475,12 +4601,12 @@
     <row r="33" spans="2:16" s="28" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B33" s="114"/>
       <c r="C33" s="44" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D33" s="44"/>
       <c r="E33" s="44"/>
       <c r="F33" s="44" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G33" s="44">
         <v>25</v>
@@ -4489,16 +4615,16 @@
         <v>25</v>
       </c>
       <c r="I33" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J33" s="43" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K33" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L33" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
@@ -4508,26 +4634,26 @@
     <row r="34" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="114"/>
       <c r="C34" s="44" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D34" s="44"/>
       <c r="E34" s="44"/>
       <c r="F34" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G34" s="46"/>
       <c r="H34" s="46"/>
       <c r="I34" s="44" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J34" s="43" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K34" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L34" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M34" s="30"/>
       <c r="N34" s="22"/>
@@ -4535,68 +4661,144 @@
       <c r="P34" s="22"/>
     </row>
     <row r="35" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="114"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
+      <c r="B35" s="112" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="44">
+        <v>8</v>
+      </c>
+      <c r="H35" s="44">
+        <v>8</v>
+      </c>
+      <c r="I35" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="J35" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="K35" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L35" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
       <c r="P35" s="22"/>
     </row>
     <row r="36" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="114"/>
-      <c r="C36" s="44"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="44" t="s">
+        <v>140</v>
+      </c>
       <c r="D36" s="44"/>
       <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
+      <c r="F36" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" s="44">
+        <v>25</v>
+      </c>
+      <c r="H36" s="44">
+        <v>25</v>
+      </c>
+      <c r="I36" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="K36" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L36" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
       <c r="P36" s="22"/>
     </row>
     <row r="37" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="114"/>
-      <c r="C37" s="44"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="44" t="s">
+        <v>154</v>
+      </c>
       <c r="D37" s="44"/>
       <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="44"/>
+      <c r="F37" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="G37" s="44">
+        <v>80</v>
+      </c>
+      <c r="H37" s="44">
+        <v>80</v>
+      </c>
+      <c r="I37" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="J37" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="K37" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L37" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
       <c r="P37" s="22"/>
     </row>
     <row r="38" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="114"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="44"/>
+      <c r="B38" s="114" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="44">
+        <v>1</v>
+      </c>
+      <c r="H38" s="44">
+        <v>10</v>
+      </c>
+      <c r="I38" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="J38" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="K38" s="45">
+        <v>0</v>
+      </c>
+      <c r="L38" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -4604,16 +4806,34 @@
     </row>
     <row r="39" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="114"/>
-      <c r="C39" s="44"/>
+      <c r="C39" s="44" t="s">
+        <v>157</v>
+      </c>
       <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
+      <c r="E39" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="44">
+        <v>90</v>
+      </c>
+      <c r="H39" s="44">
+        <v>90</v>
+      </c>
+      <c r="I39" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L39" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M39" s="30"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -4621,16 +4841,30 @@
     </row>
     <row r="40" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="114"/>
-      <c r="C40" s="44"/>
+      <c r="C40" s="44" t="s">
+        <v>158</v>
+      </c>
       <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
+      <c r="E40" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="44" t="s">
+        <v>41</v>
+      </c>
       <c r="G40" s="44"/>
       <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
+      <c r="I40" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J40" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="K40" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L40" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -4638,16 +4872,34 @@
     </row>
     <row r="41" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="114"/>
-      <c r="C41" s="44"/>
+      <c r="C41" s="44" t="s">
+        <v>159</v>
+      </c>
       <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="44"/>
+      <c r="E41" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G41" s="44">
+        <v>25</v>
+      </c>
+      <c r="H41" s="44">
+        <v>25</v>
+      </c>
+      <c r="I41" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="J41" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="K41" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L41" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -4655,16 +4907,34 @@
     </row>
     <row r="42" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="114"/>
-      <c r="C42" s="44"/>
+      <c r="C42" s="44" t="s">
+        <v>160</v>
+      </c>
       <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
+      <c r="E42" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="44">
+        <v>1</v>
+      </c>
+      <c r="H42" s="44">
+        <v>10</v>
+      </c>
+      <c r="I42" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="J42" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="K42" s="44">
+        <v>0</v>
+      </c>
+      <c r="L42" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -4672,102 +4942,218 @@
     </row>
     <row r="43" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="114"/>
-      <c r="C43" s="44"/>
+      <c r="C43" s="44" t="s">
+        <v>161</v>
+      </c>
       <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
+      <c r="E43" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="44" t="s">
+        <v>41</v>
+      </c>
       <c r="G43" s="44"/>
       <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
+      <c r="I43" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J43" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="K43" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L43" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
       <c r="P43" s="22"/>
     </row>
     <row r="44" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="114"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
+      <c r="B44" s="118" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="44">
+        <v>1</v>
+      </c>
+      <c r="H44" s="44">
+        <v>10</v>
+      </c>
+      <c r="I44" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="J44" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="K44" s="44">
+        <v>0</v>
+      </c>
+      <c r="L44" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
       <c r="P44" s="22"/>
     </row>
     <row r="45" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="114"/>
-      <c r="C45" s="44"/>
+      <c r="B45" s="118"/>
+      <c r="C45" s="44" t="s">
+        <v>170</v>
+      </c>
       <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="44"/>
+      <c r="E45" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" s="44">
+        <v>25</v>
+      </c>
+      <c r="H45" s="44">
+        <v>25</v>
+      </c>
+      <c r="I45" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="J45" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="K45" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L45" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
       <c r="P45" s="22"/>
     </row>
-    <row r="46" spans="2:16" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="44"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="32"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="29"/>
-      <c r="N46" s="29"/>
+    <row r="46" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" s="44">
+        <v>80</v>
+      </c>
+      <c r="H46" s="44">
+        <v>80</v>
+      </c>
+      <c r="I46" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="J46" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="K46" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="L46" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
     </row>
     <row r="47" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="32"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="29"/>
+      <c r="C47" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J47" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="K47" s="45"/>
+      <c r="L47" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="M47" s="22"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
     </row>
     <row r="48" spans="2:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="32"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="29"/>
-      <c r="N48" s="29"/>
-    </row>
-    <row r="49" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="32"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="29"/>
-      <c r="N49" s="29"/>
-    </row>
-    <row r="50" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="32"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-    </row>
-    <row r="51" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="45"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="22"/>
+      <c r="N48" s="22"/>
+      <c r="O48" s="22"/>
+      <c r="P48" s="22"/>
+    </row>
+    <row r="49" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="22"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="22"/>
+    </row>
+    <row r="50" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="22"/>
+    </row>
+    <row r="51" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D51" s="26"/>
       <c r="E51" s="26"/>
       <c r="I51" s="26"/>
@@ -4776,7 +5162,7 @@
       <c r="M51" s="29"/>
       <c r="N51" s="29"/>
     </row>
-    <row r="52" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" s="26"/>
       <c r="E52" s="26"/>
       <c r="I52" s="26"/>
@@ -4784,7 +5170,7 @@
       <c r="L52" s="26"/>
       <c r="M52" s="29"/>
     </row>
-    <row r="53" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="I53" s="26"/>
@@ -4793,7 +5179,7 @@
       <c r="M53" s="29"/>
       <c r="N53" s="29"/>
     </row>
-    <row r="54" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
       <c r="I54" s="26"/>
@@ -4802,7 +5188,7 @@
       <c r="M54" s="29"/>
       <c r="N54" s="29"/>
     </row>
-    <row r="55" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
       <c r="I55" s="26"/>
@@ -4811,7 +5197,7 @@
       <c r="M55" s="29"/>
       <c r="N55" s="29"/>
     </row>
-    <row r="56" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" s="26"/>
       <c r="E56" s="26"/>
       <c r="I56" s="26"/>
@@ -4820,7 +5206,7 @@
       <c r="M56" s="29"/>
       <c r="N56" s="29"/>
     </row>
-    <row r="57" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="26"/>
       <c r="E57" s="26"/>
       <c r="I57" s="26"/>
@@ -4828,7 +5214,7 @@
       <c r="L57" s="26"/>
       <c r="M57" s="29"/>
     </row>
-    <row r="58" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D58" s="26"/>
       <c r="E58" s="26"/>
       <c r="I58" s="26"/>
@@ -4836,7 +5222,7 @@
       <c r="L58" s="26"/>
       <c r="M58" s="29"/>
     </row>
-    <row r="59" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D59" s="26"/>
       <c r="E59" s="26"/>
       <c r="I59" s="26"/>
@@ -4845,7 +5231,7 @@
       <c r="M59" s="29"/>
       <c r="N59" s="29"/>
     </row>
-    <row r="60" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D60" s="26"/>
       <c r="E60" s="26"/>
       <c r="I60" s="26"/>
@@ -4853,7 +5239,7 @@
       <c r="L60" s="26"/>
       <c r="M60" s="29"/>
     </row>
-    <row r="61" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D61" s="26"/>
       <c r="E61" s="26"/>
       <c r="I61" s="26"/>
@@ -4861,7 +5247,7 @@
       <c r="L61" s="26"/>
       <c r="M61" s="29"/>
     </row>
-    <row r="62" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="26"/>
       <c r="E62" s="26"/>
       <c r="I62" s="26"/>
@@ -4870,7 +5256,7 @@
       <c r="M62" s="29"/>
       <c r="N62" s="29"/>
     </row>
-    <row r="63" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="26"/>
       <c r="E63" s="26"/>
       <c r="I63" s="26"/>
@@ -4878,7 +5264,7 @@
       <c r="L63" s="26"/>
       <c r="M63" s="29"/>
     </row>
-    <row r="64" spans="4:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="26"/>
       <c r="E64" s="26"/>
       <c r="I64" s="26"/>
@@ -24365,14 +24751,13 @@
       <c r="N2368" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="B3:B13"/>
     <mergeCell ref="B14:B23"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B43:B45"/>
     <mergeCell ref="B30:B34"/>
     <mergeCell ref="B24:B29"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B43"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -24388,7 +24773,7 @@
   </sheetPr>
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -24475,7 +24860,7 @@
   </sheetPr>
   <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>